<commit_message>
It knows the file changed, but can't display
</commit_message>
<xml_diff>
--- a/ExcelTestFile1.xlsx
+++ b/ExcelTestFile1.xlsx
@@ -21,6 +21,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>I can open the file from Github--but  I can't see the changes I made in the file</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,7 +383,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>